<commit_message>
Modify the python script
</commit_message>
<xml_diff>
--- a/redmine.xlsx
+++ b/redmine.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Project</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -67,6 +67,10 @@
   </si>
   <si>
     <t>This is a test ticket for verify build a ticket via python script, and the information is read from a excel.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Normal</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -110,11 +114,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,7 +417,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -476,8 +481,14 @@
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2">
-        <v>2</v>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="2">
+        <v>43035</v>
+      </c>
+      <c r="J2" s="2">
+        <v>43037</v>
       </c>
     </row>
   </sheetData>

</xml_diff>